<commit_message>
update AppsKey -> RCtrl
</commit_message>
<xml_diff>
--- a/Doc/Hotkey.xlsx
+++ b/Doc/Hotkey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19417" windowHeight="11130" tabRatio="758"/>
+    <workbookView windowWidth="19417" windowHeight="11130" tabRatio="758" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Windows" sheetId="2" r:id="rId1"/>
@@ -340,7 +340,7 @@
     <t>窗口 Main</t>
   </si>
   <si>
-    <t>[AppsKey]</t>
+    <t>[RCtrl]</t>
   </si>
   <si>
     <t>隐藏帮助</t>
@@ -3022,9 +3022,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -3071,14 +3071,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3108,24 +3116,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3139,22 +3162,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3177,33 +3186,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3235,31 +3235,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3271,7 +3253,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3295,7 +3283,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3307,49 +3373,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3373,43 +3403,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3618,15 +3618,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3638,6 +3629,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3676,6 +3687,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -3689,32 +3715,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3723,10 +3723,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3735,133 +3735,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5488,8 +5488,8 @@
   <sheetPr/>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showFormulas="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -6307,8 +6307,8 @@
   <sheetPr/>
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="15" customHeight="1" outlineLevelCol="5"/>

</xml_diff>